<commit_message>
change directories, brush off unnecessary files, clean repository
</commit_message>
<xml_diff>
--- a/database_template.xlsx
+++ b/database_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garci\Dropbox (UFL)\Research\XRD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garci\Dropbox (Personal)\scripts\XRD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E43D5F9C-C948-4653-9869-272924516C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEC3DFB-5ACC-4038-B3C4-08B7E2230780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="9166" xr2:uid="{301ADEBE-26A8-4A4A-BAF4-560E8A6961E6}"/>
+    <workbookView xWindow="4800" yWindow="2520" windowWidth="14400" windowHeight="6450" xr2:uid="{301ADEBE-26A8-4A4A-BAF4-560E8A6961E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,25 +48,25 @@
     <t>sample5.csv</t>
   </si>
   <si>
-    <t>example1</t>
-  </si>
-  <si>
-    <t>example2</t>
-  </si>
-  <si>
-    <t>example3</t>
-  </si>
-  <si>
-    <t>example4</t>
-  </si>
-  <si>
-    <t>example5</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>file</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>e4</t>
+  </si>
+  <si>
+    <t>e5</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -431,15 +431,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -447,7 +447,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>

</xml_diff>